<commit_message>
Effort and velocity modification from the Project Inception and Sprint Backlog 2
</commit_message>
<xml_diff>
--- a/Documentation/Sprint #2 Backlog.xlsx
+++ b/Documentation/Sprint #2 Backlog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>SPRINT BACKLOG</t>
   </si>
@@ -40,19 +40,22 @@
     <t>L</t>
   </si>
   <si>
+    <t>As a user, I need to be able to see what action a person has taken (such as create, delete)</t>
+  </si>
+  <si>
+    <t>Data classification</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
     <t>As a user, I need to be able to see the revision data being represented in the form of a pie chart</t>
   </si>
   <si>
     <t>Graphical Representation</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>As a user, I need to be able to see what action a person has taken (such as create, delete)</t>
-  </si>
-  <si>
-    <t>Data classification</t>
+    <t>As a user, I need to be able to see the action data being represented in the form of a histogram</t>
   </si>
   <si>
     <t>As a user, I need to be able to see the revision data for files within a team drive even when a folder exists in said drive</t>
@@ -61,10 +64,13 @@
     <t>Data retrieval from Drive using Drive API</t>
   </si>
   <si>
+    <t>As a developer, I need to be able to retrieve the files inside a folder</t>
+  </si>
+  <si>
     <t>As a developer, I need to be able to retrieve the number of actions that a user has made to a file</t>
   </si>
   <si>
-    <t>As a developer, I need to be able to retrieve the files inside a folder</t>
+    <t>Estimated Velocity: L</t>
   </si>
 </sst>
 </file>
@@ -149,14 +155,14 @@
       </right>
     </border>
     <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
     </border>
     <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -165,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -216,20 +222,17 @@
     <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
@@ -354,7 +357,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="15">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>10</v>
@@ -371,7 +374,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="15">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>13</v>
@@ -391,72 +394,88 @@
         <v>2.0</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="18">
+      <c r="A9" s="13">
         <v>5.0</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="15">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="19">
+      <c r="A10" s="13">
         <v>6.0</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="15">
         <v>2.0</v>
       </c>
-      <c r="D10" s="22" t="s">
-        <v>15</v>
+      <c r="D10" s="8" t="s">
+        <v>16</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="8"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="8"/>
+      <c r="A11" s="13">
+        <v>7.0</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="20">
+        <v>3.0</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="8"/>
-      <c r="C12" s="23"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" ht="15.0" customHeight="1">
-      <c r="A13" s="7"/>
-      <c r="C13" s="23"/>
+    <row r="13">
+      <c r="A13" s="8"/>
+      <c r="B13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="22"/>
       <c r="D13" s="8"/>
     </row>
-    <row r="14">
+    <row r="14" ht="15.0" customHeight="1">
       <c r="A14" s="7"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="7"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="8"/>
     </row>
     <row r="15">
-      <c r="A15" s="8"/>
+      <c r="A15" s="7"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="7"/>
     </row>
     <row r="16">
-      <c r="A16" s="7"/>
+      <c r="A16" s="8"/>
       <c r="D16" s="7"/>
     </row>
     <row r="17">
@@ -4406,6 +4425,10 @@
     <row r="1003">
       <c r="A1003" s="7"/>
       <c r="D1003" s="7"/>
+    </row>
+    <row r="1004">
+      <c r="A1004" s="7"/>
+      <c r="D1004" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>